<commit_message>
Error fixed for computing algorithm
Signed-off-by: jason <jjy714@gmail.com>
</commit_message>
<xml_diff>
--- a/data/food_data_copy.xlsx
+++ b/data/food_data_copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Projects/HCIAppProject/WFL/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D162A33-96DF-D940-9F7A-6769EBF56129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE472F5-6738-E941-AD8B-C3F5882D15A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="food_data copy (2)" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'food_data copy (2)'!$A$1:$G$538</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="595">
   <si>
     <t>id</t>
   </si>
@@ -1816,6 +1829,12 @@
   </si>
   <si>
     <t>고추바사삭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">일식 </t>
+  </si>
+  <si>
+    <t>기타</t>
   </si>
 </sst>
 </file>
@@ -2305,9 +2324,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2732,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I538"/>
+  <dimension ref="A1:L538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E348" sqref="E348"/>
+    <sheetView tabSelected="1" topLeftCell="A493" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="C525" sqref="C525"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2749,7 +2767,7 @@
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2778,7 +2796,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2801,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2824,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2847,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2870,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2893,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2915,8 +2933,15 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <f>COUNTIF(C:C, C2)</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2938,8 +2963,15 @@
       <c r="G8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8">
+        <f>COUNTIF(C:C, C6)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2961,8 +2993,15 @@
       <c r="G9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>593</v>
+      </c>
+      <c r="L9">
+        <f>COUNTIF(C:C, C29)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2984,8 +3023,15 @@
       <c r="G10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>175</v>
+      </c>
+      <c r="L10">
+        <f>COUNTIF(C:C, C457)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3007,8 +3053,11 @@
       <c r="G11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3031,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3053,8 +3102,15 @@
       <c r="G13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <f>COUNTIF(E:E,E2)</f>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3076,8 +3132,15 @@
       <c r="G14" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14">
+        <f>COUNTIF(E:E,E5)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3099,8 +3162,15 @@
       <c r="G15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15">
+        <f>COUNTIF(E:E,E27)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3121,6 +3191,9 @@
       </c>
       <c r="G16" t="b">
         <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -14749,7 +14822,7 @@
         <v>573</v>
       </c>
       <c r="C522" t="s">
-        <v>565</v>
+        <v>175</v>
       </c>
       <c r="D522" t="s">
         <v>557</v>
@@ -14772,7 +14845,7 @@
         <v>574</v>
       </c>
       <c r="C523" t="s">
-        <v>565</v>
+        <v>175</v>
       </c>
       <c r="D523" t="s">
         <v>557</v>
@@ -15062,11 +15135,9 @@
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B538" s="1" t="s">
+      <c r="B538" t="s">
         <v>592</v>
       </c>
-      <c r="C538" s="1"/>
-      <c r="F538" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>